<commit_message>
cambiati part number led
</commit_message>
<xml_diff>
--- a/Cad/bombhonor_BOM.xlsx
+++ b/Cad/bombhonor_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bombhonor\Cad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B80BB-963D-4B90-B376-A1E5E144D3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CF149A-4A93-414E-8157-A804A8156CB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{9170A209-5B0D-46F6-82F0-AE6FC39D9579}"/>
+    <workbookView xWindow="2070" yWindow="855" windowWidth="25815" windowHeight="13590" xr2:uid="{9170A209-5B0D-46F6-82F0-AE6FC39D9579}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>BLUE</t>
   </si>
   <si>
-    <t>859-LTST-C230TBKT</t>
-  </si>
-  <si>
     <t>spesa</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Qty to order</t>
+  </si>
+  <si>
+    <t>LTST-C230TBKT</t>
   </si>
 </sst>
 </file>
@@ -432,20 +432,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099DDE58-4914-4058-971B-F1AF4F243B8B}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -454,13 +457,16 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -474,8 +480,12 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>A2*$H$1</f>
+        <v>740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>31</v>
       </c>
@@ -489,8 +499,12 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="1">A3*$H$1</f>
+        <v>5735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -504,8 +518,12 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -517,10 +535,14 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -534,8 +556,12 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -544,17 +570,18 @@
         <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://www.mouser.it/ProductDetail/859-LTST-C230TBKT" xr:uid="{AB1E2883-0543-42CC-8627-58B700E390DB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>